<commit_message>
it is truly done
</commit_message>
<xml_diff>
--- a/kirby_pixel_art.xlsx
+++ b/kirby_pixel_art.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -46,19 +46,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF4500"/>
-        <bgColor rgb="00FF4500"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFFFFF"/>
-        <bgColor rgb="00FFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,13 +61,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -445,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B5:H12"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,70 +454,245 @@
     <col width="2" customWidth="1" min="13" max="13"/>
     <col width="2" customWidth="1" min="14" max="14"/>
     <col width="2" customWidth="1" min="15" max="15"/>
-    <col width="2" customWidth="1" min="16" max="16"/>
-    <col width="2" customWidth="1" min="17" max="17"/>
-    <col width="2" customWidth="1" min="18" max="18"/>
-    <col width="2" customWidth="1" min="19" max="19"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12" customHeight="1"/>
-    <row r="2" ht="12" customHeight="1"/>
-    <row r="3" ht="12" customHeight="1"/>
-    <row r="4" ht="12" customHeight="1"/>
+    <row r="1" ht="12" customHeight="1">
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="n"/>
+    </row>
+    <row r="2" ht="12" customHeight="1">
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="3" t="n"/>
+      <c r="I2" s="3" t="n"/>
+      <c r="J2" s="3" t="n"/>
+      <c r="K2" s="2" t="n"/>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
+    </row>
+    <row r="3" ht="12" customHeight="1">
+      <c r="D3" s="1" t="n"/>
+      <c r="E3" s="2" t="n"/>
+      <c r="F3" s="3" t="n"/>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="n"/>
+      <c r="J3" s="3" t="n"/>
+      <c r="K3" s="3" t="n"/>
+      <c r="L3" s="3" t="n"/>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="1" t="n"/>
+    </row>
+    <row r="4" ht="12" customHeight="1">
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="3" t="n"/>
+      <c r="F4" s="3" t="n"/>
+      <c r="G4" s="3" t="n"/>
+      <c r="H4" s="3" t="n"/>
+      <c r="I4" s="3" t="n"/>
+      <c r="J4" s="3" t="n"/>
+      <c r="K4" s="3" t="n"/>
+      <c r="L4" s="3" t="n"/>
+      <c r="M4" s="3" t="n"/>
+      <c r="N4" s="1" t="n"/>
+    </row>
     <row r="5" ht="12" customHeight="1">
-      <c r="D5" s="1" t="n"/>
-      <c r="E5" s="1" t="n"/>
-      <c r="F5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="3" t="n"/>
+      <c r="F5" s="3" t="n"/>
+      <c r="G5" s="3" t="n"/>
+      <c r="H5" s="3" t="n"/>
+      <c r="I5" s="3" t="n"/>
+      <c r="J5" s="3" t="n"/>
+      <c r="K5" s="3" t="n"/>
+      <c r="L5" s="3" t="n"/>
+      <c r="M5" s="3" t="n"/>
+      <c r="N5" s="2" t="n"/>
+      <c r="O5" s="1" t="n"/>
     </row>
     <row r="6" ht="12" customHeight="1">
-      <c r="C6" s="1" t="n"/>
-      <c r="D6" s="2" t="n"/>
-      <c r="E6" s="1" t="n"/>
-      <c r="F6" s="2" t="n"/>
-      <c r="G6" s="1" t="n"/>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" s="3" t="n"/>
+      <c r="E6" s="3" t="n"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="3" t="n"/>
+      <c r="H6" s="3" t="n"/>
+      <c r="I6" s="3" t="n"/>
+      <c r="J6" s="1" t="n"/>
+      <c r="K6" s="3" t="n"/>
+      <c r="L6" s="1" t="n"/>
+      <c r="M6" s="3" t="n"/>
+      <c r="N6" s="2" t="n"/>
+      <c r="O6" s="1" t="n"/>
     </row>
     <row r="7" ht="12" customHeight="1">
-      <c r="C7" s="1" t="n"/>
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="3" t="n"/>
       <c r="D7" s="3" t="n"/>
+      <c r="E7" s="3" t="n"/>
       <c r="F7" s="3" t="n"/>
-      <c r="G7" s="1" t="n"/>
+      <c r="G7" s="3" t="n"/>
+      <c r="H7" s="3" t="n"/>
+      <c r="I7" s="3" t="n"/>
+      <c r="J7" s="1" t="n"/>
+      <c r="K7" s="3" t="n"/>
+      <c r="L7" s="1" t="n"/>
+      <c r="M7" s="3" t="n"/>
+      <c r="N7" s="3" t="n"/>
+      <c r="O7" s="3" t="n"/>
+      <c r="P7" s="1" t="n"/>
     </row>
     <row r="8" ht="12" customHeight="1">
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="n"/>
-      <c r="G8" s="1" t="n"/>
-      <c r="H8" s="1" t="n"/>
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="3" t="n"/>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="3" t="n"/>
+      <c r="E8" s="3" t="n"/>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
+      <c r="H8" s="3" t="n"/>
+      <c r="I8" s="3" t="n"/>
+      <c r="J8" s="1" t="n"/>
+      <c r="K8" s="3" t="n"/>
+      <c r="L8" s="1" t="n"/>
+      <c r="M8" s="3" t="n"/>
+      <c r="N8" s="3" t="n"/>
+      <c r="O8" s="3" t="n"/>
+      <c r="P8" s="1" t="n"/>
     </row>
     <row r="9" ht="12" customHeight="1">
-      <c r="B9" s="1" t="n"/>
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="3" t="n"/>
       <c r="C9" s="3" t="n"/>
-      <c r="D9" s="1" t="n"/>
-      <c r="E9" s="1" t="n"/>
-      <c r="F9" s="1" t="n"/>
-      <c r="G9" s="3" t="n"/>
-      <c r="H9" s="1" t="n"/>
+      <c r="D9" s="3" t="n"/>
+      <c r="E9" s="3" t="n"/>
+      <c r="F9" s="3" t="n"/>
+      <c r="G9" s="2" t="n"/>
+      <c r="H9" s="2" t="n"/>
+      <c r="I9" s="3" t="n"/>
+      <c r="J9" s="3" t="n"/>
+      <c r="K9" s="3" t="n"/>
+      <c r="L9" s="3" t="n"/>
+      <c r="M9" s="2" t="n"/>
+      <c r="N9" s="2" t="n"/>
+      <c r="O9" s="3" t="n"/>
+      <c r="P9" s="1" t="n"/>
     </row>
     <row r="10" ht="12" customHeight="1">
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="n"/>
-      <c r="G10" s="1" t="n"/>
-      <c r="H10" s="1" t="n"/>
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="2" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="3" t="n"/>
+      <c r="E10" s="2" t="n"/>
+      <c r="F10" s="3" t="n"/>
+      <c r="G10" s="3" t="n"/>
+      <c r="H10" s="3" t="n"/>
+      <c r="I10" s="3" t="n"/>
+      <c r="J10" s="3" t="n"/>
+      <c r="K10" s="3" t="n"/>
+      <c r="L10" s="3" t="n"/>
+      <c r="M10" s="3" t="n"/>
+      <c r="N10" s="2" t="n"/>
+      <c r="O10" s="3" t="n"/>
+      <c r="P10" s="1" t="n"/>
     </row>
     <row r="11" ht="12" customHeight="1">
-      <c r="D11" s="4" t="n"/>
-      <c r="F11" s="4" t="n"/>
+      <c r="B11" s="1" t="n"/>
+      <c r="C11" s="2" t="n"/>
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="1" t="n"/>
+      <c r="F11" s="3" t="n"/>
+      <c r="G11" s="3" t="n"/>
+      <c r="H11" s="3" t="n"/>
+      <c r="I11" s="3" t="n"/>
+      <c r="J11" s="3" t="n"/>
+      <c r="K11" s="1" t="n"/>
+      <c r="L11" s="3" t="n"/>
+      <c r="M11" s="3" t="n"/>
+      <c r="N11" s="1" t="n"/>
+      <c r="O11" s="2" t="n"/>
+      <c r="P11" s="1" t="n"/>
     </row>
     <row r="12" ht="12" customHeight="1">
-      <c r="C12" s="5" t="n"/>
-      <c r="G12" s="5" t="n"/>
-    </row>
-    <row r="13" ht="12" customHeight="1"/>
-    <row r="14" ht="12" customHeight="1"/>
-    <row r="15" ht="12" customHeight="1"/>
-    <row r="16" ht="12" customHeight="1"/>
-    <row r="17" ht="12" customHeight="1"/>
-    <row r="18" ht="12" customHeight="1"/>
-    <row r="19" ht="12" customHeight="1"/>
+      <c r="C12" s="1" t="n"/>
+      <c r="D12" s="1" t="n"/>
+      <c r="E12" s="2" t="n"/>
+      <c r="F12" s="3" t="n"/>
+      <c r="G12" s="3" t="n"/>
+      <c r="H12" s="3" t="n"/>
+      <c r="I12" s="3" t="n"/>
+      <c r="J12" s="3" t="n"/>
+      <c r="K12" s="3" t="n"/>
+      <c r="L12" s="3" t="n"/>
+      <c r="M12" s="2" t="n"/>
+      <c r="N12" s="1" t="n"/>
+      <c r="O12" s="1" t="n"/>
+    </row>
+    <row r="13" ht="12" customHeight="1">
+      <c r="D13" s="1" t="n"/>
+      <c r="E13" s="1" t="n"/>
+      <c r="F13" s="2" t="n"/>
+      <c r="G13" s="2" t="n"/>
+      <c r="H13" s="3" t="n"/>
+      <c r="I13" s="3" t="n"/>
+      <c r="J13" s="3" t="n"/>
+      <c r="K13" s="3" t="n"/>
+      <c r="L13" s="2" t="n"/>
+      <c r="M13" s="1" t="n"/>
+      <c r="N13" s="1" t="n"/>
+    </row>
+    <row r="14" ht="12" customHeight="1">
+      <c r="C14" s="1" t="n"/>
+      <c r="D14" s="2" t="n"/>
+      <c r="E14" s="2" t="n"/>
+      <c r="F14" s="1" t="n"/>
+      <c r="G14" s="1" t="n"/>
+      <c r="H14" s="1" t="n"/>
+      <c r="I14" s="1" t="n"/>
+      <c r="J14" s="1" t="n"/>
+      <c r="K14" s="1" t="n"/>
+      <c r="L14" s="1" t="n"/>
+      <c r="M14" s="2" t="n"/>
+      <c r="N14" s="2" t="n"/>
+      <c r="O14" s="1" t="n"/>
+    </row>
+    <row r="15" ht="12" customHeight="1">
+      <c r="B15" s="1" t="n"/>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n"/>
+      <c r="E15" s="2" t="n"/>
+      <c r="F15" s="2" t="n"/>
+      <c r="G15" s="2" t="n"/>
+      <c r="H15" s="1" t="n"/>
+      <c r="I15" s="1" t="n"/>
+      <c r="J15" s="1" t="n"/>
+      <c r="K15" s="1" t="n"/>
+      <c r="L15" s="2" t="n"/>
+      <c r="M15" s="2" t="n"/>
+      <c r="N15" s="2" t="n"/>
+      <c r="O15" s="2" t="n"/>
+      <c r="P15" s="1" t="n"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="1" t="n"/>
+      <c r="D16" s="1" t="n"/>
+      <c r="E16" s="1" t="n"/>
+      <c r="F16" s="1" t="n"/>
+      <c r="G16" s="1" t="n"/>
+      <c r="K16" s="1" t="n"/>
+      <c r="L16" s="1" t="n"/>
+      <c r="M16" s="1" t="n"/>
+      <c r="N16" s="1" t="n"/>
+      <c r="O16" s="1" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>